<commit_message>
ajout des calculs et maj du diag de bode
</commit_message>
<xml_diff>
--- a/facicule julien/simu/Passe_Haut/filtre RC pour 1kHz.xlsx
+++ b/facicule julien/simu/Passe_Haut/filtre RC pour 1kHz.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\OneDrive\Bureau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julie\OneDrive\Documents\GitHub\ROBOT\facicule julien\simu\Passe_Haut\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D5B2B9-33F6-4EEB-BD2E-EACAAE2AD8C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA41C828-3766-4AB4-A1DE-FCE2D59C977A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0ECFEF0A-A359-4493-8D3E-D77900BDA9FD}"/>
   </bookViews>
@@ -33,6 +33,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>G(dB)</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -138,6 +155,17 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>G(dB)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -164,7 +192,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Feuil1!$C$1:$C$54</c:f>
+              <c:f>Feuil1!$C$2:$C$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
@@ -335,171 +363,171 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Feuil1!$D$1:$D$54</c:f>
+              <c:f>Feuil1!$D$2:$D$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
-                  <c:v>-60.008681549144505</c:v>
+                  <c:v>-60.000004342942646</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-53.996754516903486</c:v>
+                  <c:v>-53.979417458464908</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-50.483593565574125</c:v>
+                  <c:v>-50.457613991934231</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-47.99347442918021</c:v>
+                  <c:v>-47.958869660001966</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-46.063921147969666</c:v>
+                  <c:v>-46.020708485542954</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-44.488934606285625</c:v>
+                  <c:v>-44.437131335526452</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-43.158628610347982</c:v>
+                  <c:v>-43.098251998797458</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-42.007410901912451</c:v>
+                  <c:v>-41.93847819973557</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-40.992973135513338</c:v>
+                  <c:v>-40.915501575497579</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-40.086427475214919</c:v>
+                  <c:v>-40.000434272768629</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-34.15140352152509</c:v>
+                  <c:v>-33.981136917305022</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-30.714319399280768</c:v>
+                  <c:v>-30.461481798105851</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-28.299466958991061</c:v>
+                  <c:v>-27.965743332104296</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>-26.444385894257138</c:v>
+                  <c:v>-26.031443726201822</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-24.943092297205254</c:v>
+                  <c:v>-24.452581518752858</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>-23.68571475300568</c:v>
+                  <c:v>-23.119267661966482</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>-22.606675369490574</c:v>
+                  <c:v>-21.965906541173066</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-21.663679769620185</c:v>
+                  <c:v>-20.950185958638869</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-20.827853702762397</c:v>
+                  <c:v>-20.043213737826427</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-15.56302500730428</c:v>
+                  <c:v>-14.14973347970818</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-12.736441951403245</c:v>
+                  <c:v>-10.831839885012988</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-10.881360886689574</c:v>
+                  <c:v>-8.6033800657099384</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-9.5424250940983733</c:v>
+                  <c:v>-6.9897000433601884</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-8.5193746451691776</c:v>
+                  <c:v>-5.7723640760293016</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-7.7070176270201589</c:v>
+                  <c:v>-4.8299018838376027</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>-7.0436503619815198</c:v>
+                  <c:v>-4.0866387406381062</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-6.4902218300372869</c:v>
+                  <c:v>-3.4919355599053481</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-6.0205999130584669</c:v>
+                  <c:v>-3.0102999566398125</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-3.5218251809661871</c:v>
+                  <c:v>-0.96910013008056439</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-2.4987747320554203</c:v>
+                  <c:v>-0.45757490560675157</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-1.9382002600726664</c:v>
+                  <c:v>-0.2632893872234916</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-1.5836249208787785</c:v>
+                  <c:v>-0.17033339298780301</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>-1.3389357925490761</c:v>
+                  <c:v>-0.11899223299707719</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>-1.1598389394984456</c:v>
+                  <c:v>-8.7739243075052015E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>-1.0230504488984795</c:v>
+                  <c:v>-6.7333826589683232E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>-0.91514981116927185</c:v>
+                  <c:v>-5.3288335050670349E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>-0.82785370312429096</c:v>
+                  <c:v>-4.321373782642559E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>-0.42378598137769902</c:v>
+                  <c:v>-1.0843812922200362E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>-0.2848087822779371</c:v>
+                  <c:v>-4.8228153973810641E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>-0.2144773078246745</c:v>
+                  <c:v>-2.7134926337491396E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>-0.17200343522967809</c:v>
+                  <c:v>-1.7368305846483477E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>-0.14357169253521715</c:v>
+                  <c:v>-1.2062060399800347E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>-0.1232061740901394</c:v>
+                  <c:v>-8.8622484116057188E-4</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>-0.10790063772866286</c:v>
+                  <c:v>-6.7853211903191163E-4</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>-9.597765763051358E-2</c:v>
+                  <c:v>-5.3613293309645778E-4</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>-8.6427475648472585E-2</c:v>
+                  <c:v>-4.3427276862636089E-4</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>-4.3321235127953356E-2</c:v>
+                  <c:v>-1.0857226332825656E-4</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>-2.890481748214889E-2</c:v>
+                  <c:v>-4.8254674352119409E-5</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>-2.1687625843294887E-2</c:v>
+                  <c:v>-2.7143320295820964E-5</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>-1.7354430623655551E-2</c:v>
+                  <c:v>-1.7371744532214215E-5</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>-1.4464432381181712E-2</c:v>
+                  <c:v>-1.2063718852802955E-5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>-1.2399559047405206E-2</c:v>
+                  <c:v>-8.8631436480444377E-6</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>-1.0850581845329216E-2</c:v>
+                  <c:v>-6.7858459778732847E-6</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>-9.645630794270714E-3</c:v>
+                  <c:v>-5.3616569599545495E-6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -507,7 +535,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1DF8-4C7F-A279-771D0ADEE8E7}"/>
+              <c16:uniqueId val="{00000000-04DB-41F5-B5C2-0EEDFD60AAB9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -519,11 +547,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1736756015"/>
-        <c:axId val="1736739695"/>
+        <c:axId val="1881288256"/>
+        <c:axId val="1881282016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1736756015"/>
+        <c:axId val="1881288256"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -581,12 +609,12 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1736739695"/>
+        <c:crossAx val="1881282016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1736739695"/>
+        <c:axId val="1881282016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -643,7 +671,7 @@
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1736756015"/>
+        <c:crossAx val="1881288256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1259,23 +1287,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1">
+        <xdr:cNvPr id="3" name="Graphique 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC9C14D7-270A-6B63-C7E6-02B24173B988}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{827F347F-EAA2-99A8-CF1B-717F39D1AD24}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1613,268 +1641,277 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6599B5-BBDB-49D0-9A1D-F3342909E06F}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D54"/>
+      <selection activeCell="C1" sqref="C1:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <f>B1*10^A1</f>
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <f>20*LOG10(((1.591549431*10^(-4)*2*PI()*C1))/(1+(1.591549431*10^(-4)*2*PI()*C1)))</f>
-        <v>-60.008681549144505</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C54" si="0">B2*10^A2</f>
-        <v>2</v>
+        <f>B2*10^A2</f>
+        <v>1</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D54" si="1">20*LOG10(((1.591549431*10^(-4)*2*PI()*C2))/(1+(1.591549431*10^(-4)*2*PI()*C2)))</f>
-        <v>-53.996754516903486</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <f>20*LOG10((($G$2*$H$2*2*PI()*C2))/SQRT(1+($G$2*$H$2*2*PI()*C2)^2))</f>
+        <v>-60.000004342942646</v>
+      </c>
+      <c r="G2">
+        <f>1/(2*PI()*1000*10^(-9))</f>
+        <v>159154.94309189534</v>
+      </c>
+      <c r="H2">
+        <f>1*10^(-9)</f>
+        <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f t="shared" ref="C3:C55" si="0">B3*10^A3</f>
+        <v>2</v>
       </c>
       <c r="D3">
-        <f t="shared" si="1"/>
-        <v>-50.483593565574125</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D3:D55" si="1">20*LOG10((($G$2*$H$2*2*PI()*C3))/SQRT(1+($G$2*$H$2*2*PI()*C3)^2))</f>
+        <v>-53.979417458464908</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
-        <v>-47.99347442918021</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-50.457613991934231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
-        <v>-46.063921147969666</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-47.958869660001966</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
       <c r="B6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
-        <v>-44.488934606285625</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-46.020708485542954</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
-        <v>-43.158628610347982</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-44.437131335526452</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
-        <v>-42.007410901912451</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-43.098251998797458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
       <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>-41.93847819973557</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="1"/>
-        <v>-40.992973135513338</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>-40.086427475214919</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-40.915501575497579</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>-34.15140352152509</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-40.000434272768629</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>-30.714319399280768</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-33.981136917305022</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>-28.299466958991061</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-30.461481798105851</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>-26.444385894257138</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-27.965743332104296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
-        <v>-24.943092297205254</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-26.031443726201822</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
-        <v>-23.68571475300568</v>
+        <v>-24.452581518752858</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1882,15 +1919,15 @@
         <v>1</v>
       </c>
       <c r="B17">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
-        <v>-22.606675369490574</v>
+        <v>-23.119267661966482</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1898,31 +1935,31 @@
         <v>1</v>
       </c>
       <c r="B18">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
-        <v>-21.663679769620185</v>
+        <v>-21.965906541173066</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
-        <v>-20.827853702762397</v>
+        <v>-20.950185958638869</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1930,15 +1967,15 @@
         <v>2</v>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
-        <v>-15.56302500730428</v>
+        <v>-20.043213737826427</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1946,15 +1983,15 @@
         <v>2</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
-        <v>-12.736441951403245</v>
+        <v>-14.14973347970818</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1962,15 +1999,15 @@
         <v>2</v>
       </c>
       <c r="B22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
-        <v>-10.881360886689574</v>
+        <v>-10.831839885012988</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1978,15 +2015,15 @@
         <v>2</v>
       </c>
       <c r="B23">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>400</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
-        <v>-9.5424250940983733</v>
+        <v>-8.6033800657099384</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1994,15 +2031,15 @@
         <v>2</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>500</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>-8.5193746451691776</v>
+        <v>-6.9897000433601884</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -2010,15 +2047,15 @@
         <v>2</v>
       </c>
       <c r="B25">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
-        <v>-7.7070176270201589</v>
+        <v>-5.7723640760293016</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2026,15 +2063,15 @@
         <v>2</v>
       </c>
       <c r="B26">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
-        <v>-7.0436503619815198</v>
+        <v>-4.8299018838376027</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2042,31 +2079,31 @@
         <v>2</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
-        <v>-6.4902218300372869</v>
+        <v>-4.0866387406381062</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>900</v>
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
-        <v>-6.0205999130584669</v>
+        <v>-3.4919355599053481</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -2074,15 +2111,15 @@
         <v>3</v>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="D29">
         <f t="shared" si="1"/>
-        <v>-3.5218251809661871</v>
+        <v>-3.0102999566398125</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2090,15 +2127,15 @@
         <v>3</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="D30">
         <f t="shared" si="1"/>
-        <v>-2.4987747320554203</v>
+        <v>-0.96910013008056439</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2106,15 +2143,15 @@
         <v>3</v>
       </c>
       <c r="B31">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="D31">
         <f t="shared" si="1"/>
-        <v>-1.9382002600726664</v>
+        <v>-0.45757490560675157</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2122,15 +2159,15 @@
         <v>3</v>
       </c>
       <c r="B32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>4000</v>
       </c>
       <c r="D32">
         <f t="shared" si="1"/>
-        <v>-1.5836249208787785</v>
+        <v>-0.2632893872234916</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2138,15 +2175,15 @@
         <v>3</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>6000</v>
+        <v>5000</v>
       </c>
       <c r="D33">
         <f t="shared" si="1"/>
-        <v>-1.3389357925490761</v>
+        <v>-0.17033339298780301</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2154,15 +2191,15 @@
         <v>3</v>
       </c>
       <c r="B34">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>7000</v>
+        <v>6000</v>
       </c>
       <c r="D34">
         <f t="shared" si="1"/>
-        <v>-1.1598389394984456</v>
+        <v>-0.11899223299707719</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2170,15 +2207,15 @@
         <v>3</v>
       </c>
       <c r="B35">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>7000</v>
       </c>
       <c r="D35">
         <f t="shared" si="1"/>
-        <v>-1.0230504488984795</v>
+        <v>-8.7739243075052015E-2</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2186,31 +2223,31 @@
         <v>3</v>
       </c>
       <c r="B36">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>9000</v>
+        <v>8000</v>
       </c>
       <c r="D36">
         <f t="shared" si="1"/>
-        <v>-0.91514981116927185</v>
+        <v>-6.7333826589683232E-2</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>9000</v>
       </c>
       <c r="D37">
         <f t="shared" si="1"/>
-        <v>-0.82785370312429096</v>
+        <v>-5.3288335050670349E-2</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2218,15 +2255,15 @@
         <v>4</v>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="D38">
         <f t="shared" si="1"/>
-        <v>-0.42378598137769902</v>
+        <v>-4.321373782642559E-2</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -2234,15 +2271,15 @@
         <v>4</v>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>30000</v>
+        <v>20000</v>
       </c>
       <c r="D39">
         <f t="shared" si="1"/>
-        <v>-0.2848087822779371</v>
+        <v>-1.0843812922200362E-2</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2250,15 +2287,15 @@
         <v>4</v>
       </c>
       <c r="B40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>40000</v>
+        <v>30000</v>
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
-        <v>-0.2144773078246745</v>
+        <v>-4.8228153973810641E-3</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2266,15 +2303,15 @@
         <v>4</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>50000</v>
+        <v>40000</v>
       </c>
       <c r="D41">
         <f t="shared" si="1"/>
-        <v>-0.17200343522967809</v>
+        <v>-2.7134926337491396E-3</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -2282,15 +2319,15 @@
         <v>4</v>
       </c>
       <c r="B42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>60000</v>
+        <v>50000</v>
       </c>
       <c r="D42">
         <f t="shared" si="1"/>
-        <v>-0.14357169253521715</v>
+        <v>-1.7368305846483477E-3</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2298,15 +2335,15 @@
         <v>4</v>
       </c>
       <c r="B43">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>70000</v>
+        <v>60000</v>
       </c>
       <c r="D43">
         <f t="shared" si="1"/>
-        <v>-0.1232061740901394</v>
+        <v>-1.2062060399800347E-3</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2314,15 +2351,15 @@
         <v>4</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>80000</v>
+        <v>70000</v>
       </c>
       <c r="D44">
         <f t="shared" si="1"/>
-        <v>-0.10790063772866286</v>
+        <v>-8.8622484116057188E-4</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2330,31 +2367,31 @@
         <v>4</v>
       </c>
       <c r="B45">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
-        <v>90000</v>
+        <v>80000</v>
       </c>
       <c r="D45">
         <f t="shared" si="1"/>
-        <v>-9.597765763051358E-2</v>
+        <v>-6.7853211903191163E-4</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>90000</v>
       </c>
       <c r="D46">
         <f t="shared" si="1"/>
-        <v>-8.6427475648472585E-2</v>
+        <v>-5.3613293309645778E-4</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2362,15 +2399,15 @@
         <v>5</v>
       </c>
       <c r="B47">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>200000</v>
+        <v>100000</v>
       </c>
       <c r="D47">
         <f t="shared" si="1"/>
-        <v>-4.3321235127953356E-2</v>
+        <v>-4.3427276862636089E-4</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -2378,15 +2415,15 @@
         <v>5</v>
       </c>
       <c r="B48">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>300000</v>
+        <v>200000</v>
       </c>
       <c r="D48">
         <f t="shared" si="1"/>
-        <v>-2.890481748214889E-2</v>
+        <v>-1.0857226332825656E-4</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2394,15 +2431,15 @@
         <v>5</v>
       </c>
       <c r="B49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>400000</v>
+        <v>300000</v>
       </c>
       <c r="D49">
         <f t="shared" si="1"/>
-        <v>-2.1687625843294887E-2</v>
+        <v>-4.8254674352119409E-5</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -2410,15 +2447,15 @@
         <v>5</v>
       </c>
       <c r="B50">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>500000</v>
+        <v>400000</v>
       </c>
       <c r="D50">
         <f t="shared" si="1"/>
-        <v>-1.7354430623655551E-2</v>
+        <v>-2.7143320295820964E-5</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -2426,15 +2463,15 @@
         <v>5</v>
       </c>
       <c r="B51">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>600000</v>
+        <v>500000</v>
       </c>
       <c r="D51">
         <f t="shared" si="1"/>
-        <v>-1.4464432381181712E-2</v>
+        <v>-1.7371744532214215E-5</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -2442,15 +2479,15 @@
         <v>5</v>
       </c>
       <c r="B52">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>700000</v>
+        <v>600000</v>
       </c>
       <c r="D52">
         <f t="shared" si="1"/>
-        <v>-1.2399559047405206E-2</v>
+        <v>-1.2063718852802955E-5</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -2458,15 +2495,15 @@
         <v>5</v>
       </c>
       <c r="B53">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>800000</v>
+        <v>700000</v>
       </c>
       <c r="D53">
         <f t="shared" si="1"/>
-        <v>-1.0850581845329216E-2</v>
+        <v>-8.8631436480444377E-6</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -2474,15 +2511,31 @@
         <v>5</v>
       </c>
       <c r="B54">
+        <v>8</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>800000</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>-6.7858459778732847E-6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>5</v>
+      </c>
+      <c r="B55">
         <v>9</v>
       </c>
-      <c r="C54">
+      <c r="C55">
         <f t="shared" si="0"/>
         <v>900000</v>
       </c>
-      <c r="D54">
-        <f t="shared" si="1"/>
-        <v>-9.645630794270714E-3</v>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>-5.3616569599545495E-6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>